<commit_message>
Atualização do endereços dos lugares
</commit_message>
<xml_diff>
--- a/OBRAS DE PAVIMENTACAO-Natercio.xlsx
+++ b/OBRAS DE PAVIMENTACAO-Natercio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAMSUNG\Desktop\apresentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D261922D-E118-4F8E-A6B5-7E4A4101E875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EC17A2-BE2A-43BD-8431-AB936D4331BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="769" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +526,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -640,7 +648,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -749,6 +757,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1035,8 +1046,8 @@
   <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2058,7 @@
       <c r="C24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="35" t="s">
         <v>80</v>
       </c>
       <c r="E24" s="18">
@@ -2087,7 +2098,7 @@
       <c r="C25" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="35" t="s">
         <v>77</v>
       </c>
       <c r="E25" s="18">
@@ -2127,7 +2138,7 @@
       <c r="C26" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="35" t="s">
         <v>78</v>
       </c>
       <c r="E26" s="18">
@@ -2167,7 +2178,7 @@
       <c r="C27" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="35" t="s">
         <v>85</v>
       </c>
       <c r="E27" s="18">
@@ -2207,7 +2218,7 @@
       <c r="C28" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="35" t="s">
         <v>79</v>
       </c>
       <c r="E28" s="18">
@@ -2247,7 +2258,7 @@
       <c r="C29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="35" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="18">
@@ -2293,7 +2304,7 @@
       <c r="C30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="35" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="18">
@@ -2339,7 +2350,7 @@
       <c r="C31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="35" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="18">
@@ -2379,7 +2390,7 @@
       <c r="C32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="35" t="s">
         <v>50</v>
       </c>
       <c r="E32" s="18">
@@ -2419,7 +2430,7 @@
       <c r="C33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="35" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="18">
@@ -2459,7 +2470,7 @@
       <c r="C34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="35" t="s">
         <v>65</v>
       </c>
       <c r="E34" s="18">
@@ -2499,7 +2510,7 @@
       <c r="C35" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="35" t="s">
         <v>95</v>
       </c>
       <c r="E35" s="22">
@@ -2545,7 +2556,7 @@
       <c r="C36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="35" t="s">
         <v>108</v>
       </c>
       <c r="E36" s="22">
@@ -2585,7 +2596,7 @@
       <c r="C37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="35" t="s">
         <v>94</v>
       </c>
       <c r="E37" s="22">
@@ -2631,7 +2642,7 @@
       <c r="C38" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="35" t="s">
         <v>134</v>
       </c>
       <c r="E38" s="22">
@@ -2671,7 +2682,7 @@
       <c r="C39" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="35" t="s">
         <v>135</v>
       </c>
       <c r="E39" s="22">
@@ -2711,7 +2722,7 @@
       <c r="C40" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="35" t="s">
         <v>136</v>
       </c>
       <c r="E40" s="22">
@@ -2751,7 +2762,7 @@
       <c r="C41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="36" t="s">
         <v>63</v>
       </c>
       <c r="E41" s="18">
@@ -2797,7 +2808,7 @@
       <c r="C42" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="36" t="s">
         <v>129</v>
       </c>
       <c r="E42" s="18">
@@ -2837,7 +2848,7 @@
       <c r="C43" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="36" t="s">
         <v>109</v>
       </c>
       <c r="E43" s="18">
@@ -2877,7 +2888,7 @@
       <c r="C44" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="36" t="s">
         <v>132</v>
       </c>
       <c r="E44" s="18">
@@ -2917,7 +2928,7 @@
       <c r="C45" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="36" t="s">
         <v>130</v>
       </c>
       <c r="E45" s="18">
@@ -2957,7 +2968,7 @@
       <c r="C46" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="36" t="s">
         <v>131</v>
       </c>
       <c r="E46" s="18">
@@ -2997,7 +3008,7 @@
       <c r="C47" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="35" t="s">
         <v>45</v>
       </c>
       <c r="E47" s="18">
@@ -3037,7 +3048,7 @@
       <c r="C48" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="35" t="s">
         <v>60</v>
       </c>
       <c r="E48" s="18">
@@ -3077,7 +3088,7 @@
       <c r="C49" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="34" t="s">
         <v>59</v>
       </c>
       <c r="E49" s="17">
@@ -3117,7 +3128,7 @@
       <c r="C50" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="35" t="s">
         <v>61</v>
       </c>
       <c r="E50" s="17">
@@ -3157,7 +3168,7 @@
       <c r="C51" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="35" t="s">
         <v>62</v>
       </c>
       <c r="E51" s="17">
@@ -3197,7 +3208,7 @@
       <c r="C52" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="D52" s="35" t="s">
         <v>109</v>
       </c>
       <c r="E52" s="26">
@@ -3239,7 +3250,7 @@
       <c r="C53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="34" t="s">
         <v>71</v>
       </c>
       <c r="E53" s="17">
@@ -3278,7 +3289,7 @@
       <c r="C54" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="35" t="s">
         <v>73</v>
       </c>
       <c r="E54" s="17">
@@ -3318,7 +3329,7 @@
       <c r="C55" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="35" t="s">
         <v>74</v>
       </c>
       <c r="E55" s="17">
@@ -3358,7 +3369,7 @@
       <c r="C56" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="35" t="s">
         <v>72</v>
       </c>
       <c r="E56" s="17">
@@ -3398,7 +3409,7 @@
       <c r="C57" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="37" t="s">
         <v>30</v>
       </c>
       <c r="E57" s="17">

</xml_diff>

<commit_message>
Atualização de mtade dos endereços
</commit_message>
<xml_diff>
--- a/OBRAS DE PAVIMENTACAO-Natercio.xlsx
+++ b/OBRAS DE PAVIMENTACAO-Natercio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAMSUNG\Desktop\apresentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EC17A2-BE2A-43BD-8431-AB936D4331BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38543EB1-6C8C-4328-B3F8-DFA940247880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="769" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -758,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1046,8 +1046,8 @@
   <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3449,7 +3449,7 @@
       <c r="C58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="35" t="s">
         <v>44</v>
       </c>
       <c r="E58" s="17">
@@ -3495,7 +3495,7 @@
       <c r="C59" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="35" t="s">
         <v>46</v>
       </c>
       <c r="E59" s="18">
@@ -3535,7 +3535,7 @@
       <c r="C60" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="35" t="s">
         <v>57</v>
       </c>
       <c r="E60" s="17">
@@ -3575,7 +3575,7 @@
       <c r="C61" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="35" t="s">
         <v>31</v>
       </c>
       <c r="E61" s="18">
@@ -3615,7 +3615,7 @@
       <c r="C62" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="35" t="s">
         <v>56</v>
       </c>
       <c r="E62" s="18">

</xml_diff>